<commit_message>
UI update, modify leaderboard and user manager
</commit_message>
<xml_diff>
--- a/user&pass.xlsx
+++ b/user&pass.xlsx
@@ -1,64 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cuhk\hci\proj\justmove-master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF330EED-244F-46B9-8C49-5C5D6E1B4CCE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
   <si>
+    <t>5F4DCC3B5AA765D61D8327DEB882CF99</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>5F4DCC3B5AA765D61D8327DEB882CF99</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>21232F297A57A5A743894A0E4A801FC3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>d8578edf8458ce06fbc5bb76a58c5ca4</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>202cb962ac59075b964b07152d234b70</t>
+  </si>
+  <si>
+    <t>username1</t>
+  </si>
+  <si>
+    <t>qwe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -74,24 +78,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -379,34 +374,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="2" min="2" width="43.33203125"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rewrite user manager, combine leaderboard
</commit_message>
<xml_diff>
--- a/user&pass.xlsx
+++ b/user&pass.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>qwe</t>
+  </si>
+  <si>
+    <t>d41d8cd98f00b204e9800998ecf8427e</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="A4:D4"/>
@@ -456,6 +459,15 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s"/>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>

</xml_diff>